<commit_message>
Updated Script for UI automation
</commit_message>
<xml_diff>
--- a/src/test/java/Data/ShoppingCartTestdata.xlsx
+++ b/src/test/java/Data/ShoppingCartTestdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\Demo\src\test\java\TestFeatureFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DemoTCBProject\Demoframework\src\test\java\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{097F31DF-1478-42F3-9AD1-F95F31AC4E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33FC568-1310-41DE-985F-758A78EADDEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{91B4F57A-CB8D-468D-A272-112603FCE22B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{91B4F57A-CB8D-468D-A272-112603FCE22B}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>ZipCode</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>$32.39</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
   </si>
 </sst>
 </file>
@@ -114,8 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,12 +469,13 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -484,36 +486,36 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1">
         <v>214258</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>